<commit_message>
Fixed some variables. Ran a few more simulations, and now have FBA fluxes_allrxns for all 6 weights.
</commit_message>
<xml_diff>
--- a/matlab/MeCorr/VariablesSaved/sigRxnT_6FBA.xlsx
+++ b/matlab/MeCorr/VariablesSaved/sigRxnT_6FBA.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\Documents\CancerMetabRes\egem-lf\matlab\MeCorr\VariablesSaved\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE704CC3-42AB-4EC5-80E7-F25E9D430659}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B4F77A-718E-4509-B897-9B6D8DA76A3B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10335" yWindow="2250" windowWidth="10155" windowHeight="7875" xr2:uid="{53E2718A-87F7-439C-9FAC-3321167CA815}"/>
+    <workbookView xWindow="1365" yWindow="2775" windowWidth="10155" windowHeight="7875" xr2:uid="{53E2718A-87F7-439C-9FAC-3321167CA815}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
@@ -550,7 +548,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78DB7B2-85A9-44AA-8B28-6BC4C2840399}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1141,28 +1141,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16361D40-9478-476D-8FDC-02D543D14494}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8103E6A1-261B-4815-9383-A7579ECC6C62}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>